<commit_message>
Test : view Test
</commit_message>
<xml_diff>
--- a/file/CSV/Product_example.xlsx
+++ b/file/CSV/Product_example.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gamja file\fulfillmentBlue\file\CSV\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E98807-78FF-4E6C-813A-E75F84F0C04A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{569EF7D9-465C-40C9-A11B-1CC5A44065B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,430 +42,432 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>A101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A103</t>
+  </si>
+  <si>
+    <t>A104</t>
+  </si>
+  <si>
+    <t>A105</t>
+  </si>
+  <si>
+    <t>A106</t>
+  </si>
+  <si>
+    <t>A107</t>
+  </si>
+  <si>
+    <t>A108</t>
+  </si>
+  <si>
+    <t>A109</t>
+  </si>
+  <si>
+    <t>삼겹살 500g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돼지갈비 500g(구이용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돼지갈비 1kg(찜용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돼지등심 500g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A110</t>
+  </si>
+  <si>
+    <t>A111</t>
+  </si>
+  <si>
+    <t>소고기 스테이크 set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B102</t>
+  </si>
+  <si>
+    <t>B103</t>
+  </si>
+  <si>
+    <t>B104</t>
+  </si>
+  <si>
+    <t>B105</t>
+  </si>
+  <si>
+    <t>B106</t>
+  </si>
+  <si>
+    <t>B107</t>
+  </si>
+  <si>
+    <t>소시지 10개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닭꼬치 10개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양꼬치 10개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돼지고기 꼬치 10개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새우꼬치 10개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>야채꼬치 10개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모듬꼬치 각 2개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C103</t>
+  </si>
+  <si>
+    <t>C104</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>C106</t>
+  </si>
+  <si>
+    <t>C107</t>
+  </si>
+  <si>
+    <t>연어 300g(스테이크용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>립아이 300g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>티본스테이크 300g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토마호크 300g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>찹스테이크 300g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이크용 부위 300g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고베 스테이크용 부위 300g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>굴 1kg(구이용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>농어 300g(스테이크용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숭어 1마리(구이용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍합 1kg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새우 10마리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가리비 1kg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대개 1kg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D102</t>
+  </si>
+  <si>
+    <t>D103</t>
+  </si>
+  <si>
+    <t>D104</t>
+  </si>
+  <si>
+    <t>D105</t>
+  </si>
+  <si>
+    <t>D106</t>
+  </si>
+  <si>
+    <t>D107</t>
+  </si>
+  <si>
+    <t>D108</t>
+  </si>
+  <si>
+    <t>D109</t>
+  </si>
+  <si>
+    <t>아스파라거스 5개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방울토마토 500g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가지 2개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마늘 300g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대파 1단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양파 5개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레몬 1개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파프리카 2개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양송이버섯 100g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E102</t>
+  </si>
+  <si>
+    <t>E103</t>
+  </si>
+  <si>
+    <t>E104</t>
+  </si>
+  <si>
+    <t>E105</t>
+  </si>
+  <si>
+    <t>E106</t>
+  </si>
+  <si>
+    <t>고추 100g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시나몬가루 100g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월계수 잎 50g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통후추 100g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로즈마리 50g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>향신료 세트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>../img/meat/pork_belly.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/pork_rib.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/pork_rib_steak.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/pork_loin.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/ribeye.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/T-bone steak.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/Tomahawk.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/chap_beef.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/beef_steak.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/gobe_beef.jpg</t>
+  </si>
+  <si>
+    <t>../img/meat/beef_set.jpg</t>
+  </si>
+  <si>
+    <t>B108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>../img/seafood/salmon_steak.jpg</t>
+  </si>
+  <si>
+    <t>../img/seafood/bass.jpg</t>
+  </si>
+  <si>
+    <t>../img/seafood/sea_bream.jpg</t>
+  </si>
+  <si>
+    <t>../img/seafood/oysters.jpg</t>
+  </si>
+  <si>
+    <t>../img/seafood/mussels.jpg</t>
+  </si>
+  <si>
+    <t>../img/seafood/scallop.jpg</t>
+  </si>
+  <si>
+    <t>../img/seafood/shrimp.jpg</t>
+  </si>
+  <si>
+    <t>../img/seafood/snow_crab.jpg</t>
+  </si>
+  <si>
+    <t>../img/BBQ/sausage.jpg</t>
+  </si>
+  <si>
+    <t>../img/BBQ/skewered_chicken.jpg</t>
+  </si>
+  <si>
+    <t>../img/BBQ/skewered_lamb.jpg</t>
+  </si>
+  <si>
+    <t>../img/BBQ/skewered_pork.jpg</t>
+  </si>
+  <si>
+    <t>../img/BBQ/skewered_shrimp.jpg</t>
+  </si>
+  <si>
+    <t>../img/BBQ/skewered_vegetable.jpg</t>
+  </si>
+  <si>
+    <t>../img/BBQ/skewered_set.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/asparagus.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/cherry_tomato.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/eggplant.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/garlic.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/green_onion.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/onion.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/lemon.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/paprika.jpg</t>
+  </si>
+  <si>
+    <t>../img/vegetable/white_mushroom.jpg</t>
+  </si>
+  <si>
+    <t>../img/spicy/chili.jpg</t>
+  </si>
+  <si>
+    <t>../img/spicy/cinnamon.jpg</t>
+  </si>
+  <si>
+    <t>../img/spicy/laurel.jpg</t>
+  </si>
+  <si>
+    <t>../img/spicy/papper.jpg</t>
+  </si>
+  <si>
+    <t>../img/spicy/rosemary.jpg</t>
+  </si>
+  <si>
+    <t>../img/spicy/spices_set.jpg</t>
+  </si>
+  <si>
     <t>이미지 경로</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A103</t>
-  </si>
-  <si>
-    <t>A104</t>
-  </si>
-  <si>
-    <t>A105</t>
-  </si>
-  <si>
-    <t>A106</t>
-  </si>
-  <si>
-    <t>A107</t>
-  </si>
-  <si>
-    <t>A108</t>
-  </si>
-  <si>
-    <t>A109</t>
-  </si>
-  <si>
-    <t>삼겹살 500g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돼지갈비 500g(구이용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돼지갈비 1kg(찜용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돼지등심 500g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A110</t>
-  </si>
-  <si>
-    <t>A111</t>
-  </si>
-  <si>
-    <t>소고기 스테이크 set</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B102</t>
-  </si>
-  <si>
-    <t>B103</t>
-  </si>
-  <si>
-    <t>B104</t>
-  </si>
-  <si>
-    <t>B105</t>
-  </si>
-  <si>
-    <t>B106</t>
-  </si>
-  <si>
-    <t>B107</t>
-  </si>
-  <si>
-    <t>소시지 10개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>닭꼬치 10개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>양꼬치 10개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돼지고기 꼬치 10개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새우꼬치 10개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>야채꼬치 10개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모듬꼬치 각 2개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C102</t>
-  </si>
-  <si>
-    <t>C103</t>
-  </si>
-  <si>
-    <t>C104</t>
-  </si>
-  <si>
-    <t>C105</t>
-  </si>
-  <si>
-    <t>C106</t>
-  </si>
-  <si>
-    <t>C107</t>
-  </si>
-  <si>
-    <t>C108</t>
-  </si>
-  <si>
-    <t>연어 300g(스테이크용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>립아이 300g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>티본스테이크 300g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>토마호크 300g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>찹스테이크 300g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스테이크용 부위 300g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고베 스테이크용 부위 300g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>굴 1kg(구이용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>농어 300g(스테이크용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>숭어 1마리(구이용)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>홍합 1kg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새우 10마리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가리비 1kg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대개 1kg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D102</t>
-  </si>
-  <si>
-    <t>D103</t>
-  </si>
-  <si>
-    <t>D104</t>
-  </si>
-  <si>
-    <t>D105</t>
-  </si>
-  <si>
-    <t>D106</t>
-  </si>
-  <si>
-    <t>D107</t>
-  </si>
-  <si>
-    <t>D108</t>
-  </si>
-  <si>
-    <t>D109</t>
-  </si>
-  <si>
-    <t>아스파라거스 5개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방울토마토 500g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가지 2개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마늘 300g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대파 1단</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>양파 5개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>레몬 1개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파프리카 2개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>양송이버섯 100g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E102</t>
-  </si>
-  <si>
-    <t>E103</t>
-  </si>
-  <si>
-    <t>E104</t>
-  </si>
-  <si>
-    <t>E105</t>
-  </si>
-  <si>
-    <t>E106</t>
-  </si>
-  <si>
-    <t>고추 100g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시나몬가루 100g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월계수 잎 50g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>통후추 100g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로즈마리 50g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>향신료 세트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>../img/meatpork_belly.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatpork_rib.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatpork_rib_steak.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatpork_loin.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatribeye.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatT-bone steak.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatTomahawk.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatchap_beef.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatbeef_steak.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatgobe_beef.jpg</t>
-  </si>
-  <si>
-    <t>../img/meatbeef_set.jpg</t>
-  </si>
-  <si>
-    <t>../img/seafoodsausage.jpg</t>
-  </si>
-  <si>
-    <t>../img/seafoodskewered_chicken.jpg</t>
-  </si>
-  <si>
-    <t>../img/seafoodskewered_lamb.jpg</t>
-  </si>
-  <si>
-    <t>../img/seafoodskewered_pork.jpg</t>
-  </si>
-  <si>
-    <t>../img/seafoodskewered_shrimp.jpg</t>
-  </si>
-  <si>
-    <t>../img/seafoodskewered_vegetable.jpg</t>
-  </si>
-  <si>
-    <t>../img/seafoodskewered_set.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQsalmon_steak.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQbass.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQsea_bream.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQoysters.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQmussels.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQscallop.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQshrimp.jpg</t>
-  </si>
-  <si>
-    <t>../img/BBQsnow_crab.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetableasparagus.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetablecherry_tomato.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetableeggplant.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetablegarlic.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetablegreen_onion.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetableonion.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetablelemon.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetablepaprika.jpg</t>
-  </si>
-  <si>
-    <t>../img/vegetablewhite_mushroom.jpg</t>
-  </si>
-  <si>
-    <t>../img/spicychili.jpg</t>
-  </si>
-  <si>
-    <t>../img/spicycinnamon.jpg</t>
-  </si>
-  <si>
-    <t>../img/spicylaurel.jpg</t>
-  </si>
-  <si>
-    <t>../img/spicypapper.jpg</t>
-  </si>
-  <si>
-    <t>../img/spicyrosemary.jpg</t>
-  </si>
-  <si>
-    <t>../img/spicyspices_set.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,8 +515,36 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -821,26 +845,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022B68C0-EA1D-48FB-BDA1-ABE917892CFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -857,15 +879,15 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>7000</v>
@@ -874,15 +896,15 @@
         <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>13000</v>
@@ -891,15 +913,15 @@
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>10000</v>
@@ -908,15 +930,15 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>5000</v>
@@ -925,15 +947,15 @@
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>10000</v>
@@ -942,15 +964,15 @@
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C7">
         <v>13000</v>
@@ -959,15 +981,15 @@
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>15000</v>
@@ -976,15 +998,15 @@
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>13000</v>
@@ -993,15 +1015,15 @@
         <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>10000</v>
@@ -1010,15 +1032,15 @@
         <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>15000</v>
@@ -1027,15 +1049,15 @@
         <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
       </c>
       <c r="C12">
         <v>20000</v>
@@ -1044,32 +1066,32 @@
         <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C13">
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C14">
         <v>6000</v>
@@ -1078,32 +1100,32 @@
         <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C15">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="D15">
         <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C16">
         <v>8000</v>
@@ -1112,49 +1134,49 @@
         <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C17">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="D17">
         <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C18">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="D18">
         <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>8000</v>
@@ -1163,32 +1185,32 @@
         <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C20">
-        <v>7000</v>
+        <v>20000</v>
       </c>
       <c r="D20">
         <v>100</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>6000</v>
@@ -1197,15 +1219,15 @@
         <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>6000</v>
@@ -1214,49 +1236,49 @@
         <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C23">
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="D23">
         <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C24">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="D24">
         <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>8000</v>
@@ -1265,49 +1287,49 @@
         <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C26">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="D26">
         <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C27">
-        <v>20000</v>
+        <v>8000</v>
       </c>
       <c r="D27">
         <v>100</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C28">
         <v>3000</v>
@@ -1316,15 +1338,15 @@
         <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C29">
         <v>5000</v>
@@ -1333,15 +1355,15 @@
         <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <v>2000</v>
@@ -1350,15 +1372,15 @@
         <v>100</v>
       </c>
       <c r="E30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C31">
         <v>3000</v>
@@ -1367,15 +1389,15 @@
         <v>100</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C32">
         <v>3000</v>
@@ -1384,15 +1406,15 @@
         <v>100</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C33">
         <v>4000</v>
@@ -1401,15 +1423,15 @@
         <v>100</v>
       </c>
       <c r="E33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C34">
         <v>500</v>
@@ -1418,15 +1440,15 @@
         <v>100</v>
       </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C35">
         <v>2000</v>
@@ -1435,15 +1457,15 @@
         <v>100</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C36">
         <v>2000</v>
@@ -1452,15 +1474,15 @@
         <v>100</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <v>3000</v>
@@ -1469,15 +1491,15 @@
         <v>100</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38">
         <v>3000</v>
@@ -1486,15 +1508,15 @@
         <v>100</v>
       </c>
       <c r="E38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C39">
         <v>3000</v>
@@ -1503,15 +1525,15 @@
         <v>100</v>
       </c>
       <c r="E39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C40">
         <v>3000</v>
@@ -1520,15 +1542,15 @@
         <v>100</v>
       </c>
       <c r="E40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C41">
         <v>3000</v>
@@ -1537,15 +1559,15 @@
         <v>100</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C42">
         <v>5000</v>
@@ -1554,7 +1576,7 @@
         <v>100</v>
       </c>
       <c r="E42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>